<commit_message>
fom and vom costs implemented
</commit_message>
<xml_diff>
--- a/spine_projects/01_input_data/01_input_raw/Model_Data_Base.xlsx
+++ b/spine_projects/01_input_data/01_input_raw/Model_Data_Base.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/dahe23af_student_cbs_dk/Documents/Dokumente/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{EC3853F5-0F8A-4751-B92B-6D63D45C6909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{22F8222D-841C-40B5-BF60-1997CF88FB3F}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="13_ncr:1_{EC3853F5-0F8A-4751-B92B-6D63D45C6909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{28FF5C0C-62DF-4413-90ED-0446652C9561}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-3015" yWindow="-16200" windowWidth="23505" windowHeight="15585" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="55">
   <si>
     <t>Unit</t>
   </si>
@@ -67,12 +67,6 @@
     <t>Cost_invest</t>
   </si>
   <si>
-    <t>Cost_OM</t>
-  </si>
-  <si>
-    <t>Cost_var</t>
-  </si>
-  <si>
     <t>CO2_Vaporizer</t>
   </si>
   <si>
@@ -205,10 +199,10 @@
     <t>connection_type_normal</t>
   </si>
   <si>
-    <t>Cost_FOM (yearly)</t>
-  </si>
-  <si>
-    <t>Cost_VOM (per unit)</t>
+    <t>vom_cost</t>
+  </si>
+  <si>
+    <t>fom_cost</t>
   </si>
 </sst>
 </file>
@@ -303,8 +297,8 @@
     <tableColumn id="20" xr3:uid="{84C680FD-12EA-4AE2-A238-57453A3D8C12}" name="Relation_In_Out"/>
     <tableColumn id="10" xr3:uid="{ACDE4024-BCA2-4145-B3BC-1A5A08F3EA7D}" name="Relation_Out_Out"/>
     <tableColumn id="11" xr3:uid="{8AEC88A1-B64A-43A2-AC89-3B27AB4ACAD7}" name="Cost_invest"/>
-    <tableColumn id="12" xr3:uid="{F1A83AF0-CF23-4B00-9076-4E28DF8DAFD3}" name="Cost_FOM (yearly)"/>
-    <tableColumn id="13" xr3:uid="{AD4231E3-CB94-4597-81A2-E13C044BBD2D}" name="Cost_VOM (per unit)"/>
+    <tableColumn id="12" xr3:uid="{F1A83AF0-CF23-4B00-9076-4E28DF8DAFD3}" name="fom_cost"/>
+    <tableColumn id="13" xr3:uid="{AD4231E3-CB94-4597-81A2-E13C044BBD2D}" name="vom_cost"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -334,8 +328,8 @@
     <tableColumn id="10" xr3:uid="{AE158189-8F74-4D1A-BE7F-20B56DC1FCA0}" name="Relation_Out_Out"/>
     <tableColumn id="23" xr3:uid="{C3B5D3DD-6B9E-4750-8098-2BDCA6D4F76B}" name="Relation_Out_In"/>
     <tableColumn id="11" xr3:uid="{ADDA3F91-13EA-44FD-BDAD-129E45FF1B77}" name="Cost_invest"/>
-    <tableColumn id="12" xr3:uid="{19693C8E-93B1-45BA-838A-11FFE3971C45}" name="Cost_OM"/>
-    <tableColumn id="13" xr3:uid="{9A50D747-7636-48C7-AEA4-AC76517E91C7}" name="Cost_var"/>
+    <tableColumn id="12" xr3:uid="{19693C8E-93B1-45BA-838A-11FFE3971C45}" name="fom_cost"/>
+    <tableColumn id="13" xr3:uid="{9A50D747-7636-48C7-AEA4-AC76517E91C7}" name="vom_cost"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -355,8 +349,8 @@
     <tableColumn id="3" xr3:uid="{11AD2EA9-CE36-4CCE-8F89-387EFE0D8EED}" name="frac_state_loss"/>
     <tableColumn id="7" xr3:uid="{FDFFF561-E931-46C6-8D90-30C5BF9CB9E9}" name="node_state"/>
     <tableColumn id="11" xr3:uid="{3C880482-B284-4120-859D-C69724716B06}" name="Cost_invest"/>
-    <tableColumn id="12" xr3:uid="{DC155748-1945-4E24-B8A1-527B52E12445}" name="Cost_OM"/>
-    <tableColumn id="13" xr3:uid="{620A5657-4B04-4066-87F7-215E607C4C88}" name="Cost_var"/>
+    <tableColumn id="12" xr3:uid="{DC155748-1945-4E24-B8A1-527B52E12445}" name="fom_cost"/>
+    <tableColumn id="13" xr3:uid="{620A5657-4B04-4066-87F7-215E607C4C88}" name="vom_cost"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -661,8 +655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
   <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T4" sqref="T4"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -682,8 +676,8 @@
     <col min="16" max="16" width="17.1796875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="18.81640625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="12.7265625" customWidth="1"/>
-    <col min="19" max="19" width="18.6328125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20.6328125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.35">
@@ -703,57 +697,57 @@
         <v>5</v>
       </c>
       <c r="F1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" t="s">
         <v>30</v>
       </c>
-      <c r="G1" t="s">
-        <v>32</v>
-      </c>
       <c r="H1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" t="s">
         <v>33</v>
       </c>
-      <c r="I1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" t="s">
         <v>35</v>
-      </c>
-      <c r="K1" t="s">
-        <v>38</v>
-      </c>
-      <c r="L1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M1" t="s">
-        <v>37</v>
       </c>
       <c r="N1" t="s">
         <v>7</v>
       </c>
       <c r="O1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="P1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q1" t="s">
         <v>40</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>42</v>
       </c>
       <c r="R1" t="s">
         <v>8</v>
       </c>
       <c r="S1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="T1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J2">
         <v>304</v>
@@ -770,16 +764,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F3">
         <v>52</v>
@@ -796,13 +790,13 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J4">
         <v>100</v>
@@ -816,13 +810,13 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G5">
         <v>52</v>
@@ -837,19 +831,19 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
         <v>13</v>
       </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" t="s">
-        <v>15</v>
-      </c>
       <c r="E6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="J6">
         <v>100</v>
@@ -887,8 +881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C870BDA0-9E4C-481D-87BE-9D47789809C8}">
   <dimension ref="A1:V5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S2" sqref="S2"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="U1" sqref="U1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -910,13 +904,13 @@
     <col min="18" max="18" width="18.81640625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="18.81640625" customWidth="1"/>
     <col min="20" max="20" width="12.7265625" customWidth="1"/>
-    <col min="21" max="21" width="10.6328125" customWidth="1"/>
-    <col min="22" max="22" width="10.08984375" customWidth="1"/>
+    <col min="21" max="21" width="11" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -931,75 +925,75 @@
         <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" t="s">
         <v>30</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" t="s">
         <v>32</v>
       </c>
-      <c r="I1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J1" t="s">
-        <v>31</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N1" t="s">
         <v>35</v>
-      </c>
-      <c r="L1" t="s">
-        <v>34</v>
-      </c>
-      <c r="M1" t="s">
-        <v>36</v>
-      </c>
-      <c r="N1" t="s">
-        <v>37</v>
       </c>
       <c r="O1" t="s">
         <v>7</v>
       </c>
       <c r="P1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="Q1" t="s">
+        <v>38</v>
+      </c>
+      <c r="R1" t="s">
         <v>40</v>
       </c>
-      <c r="R1" t="s">
-        <v>42</v>
-      </c>
       <c r="S1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="T1" t="s">
         <v>8</v>
       </c>
       <c r="U1" t="s">
-        <v>9</v>
+        <v>54</v>
       </c>
       <c r="V1" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" t="s">
-        <v>19</v>
-      </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G2">
         <v>1000</v>
@@ -1028,25 +1022,28 @@
       <c r="S2">
         <v>1</v>
       </c>
+      <c r="U2">
+        <v>100</v>
+      </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I3">
         <v>1000</v>
@@ -1063,25 +1060,28 @@
       <c r="S3">
         <v>1</v>
       </c>
+      <c r="V3">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I4">
         <v>1000</v>
@@ -1101,16 +1101,16 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
         <v>22</v>
       </c>
-      <c r="B5" t="s">
-        <v>24</v>
-      </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G5">
         <v>1000</v>
@@ -1142,7 +1142,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1155,45 +1155,45 @@
     <col min="6" max="6" width="15.81640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.81640625" customWidth="1"/>
     <col min="8" max="8" width="9" customWidth="1"/>
-    <col min="9" max="9" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" t="s">
         <v>46</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>47</v>
-      </c>
-      <c r="F1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G1" t="s">
-        <v>49</v>
       </c>
       <c r="H1" t="s">
         <v>8</v>
       </c>
       <c r="I1" t="s">
-        <v>9</v>
+        <v>54</v>
       </c>
       <c r="J1" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1208,12 +1208,15 @@
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>52</v>
+        <v>50</v>
+      </c>
+      <c r="I2">
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1228,7 +1231,10 @@
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>52</v>
+        <v>50</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adjust vom_cost code in data prep
change the data prep for vom cost of unit relations
</commit_message>
<xml_diff>
--- a/spine_projects/01_input_data/01_input_raw/Model_Data_Base.xlsx
+++ b/spine_projects/01_input_data/01_input_raw/Model_Data_Base.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/dahe23af_student_cbs_dk/Documents/Dokumente/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="13_ncr:1_{EC3853F5-0F8A-4751-B92B-6D63D45C6909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{28FF5C0C-62DF-4413-90ED-0446652C9561}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2732DB53-37E9-4CEE-A7DE-12C475AEA06D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3015" yWindow="-16200" windowWidth="23505" windowHeight="15585" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-5070" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="61">
   <si>
     <t>Unit</t>
   </si>
@@ -203,6 +203,24 @@
   </si>
   <si>
     <t>fom_cost</t>
+  </si>
+  <si>
+    <t>vom_cost_input1</t>
+  </si>
+  <si>
+    <t>vom_cost_output1</t>
+  </si>
+  <si>
+    <t>vom_cost_Input1</t>
+  </si>
+  <si>
+    <t>vom_cost_Input2</t>
+  </si>
+  <si>
+    <t>vom_cost_Output1</t>
+  </si>
+  <si>
+    <t>vom_cost_Output2</t>
   </si>
 </sst>
 </file>
@@ -276,9 +294,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}" name="Table1" displayName="Table1" ref="A1:T6" totalsRowShown="0">
-  <autoFilter ref="A1:T6" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
-  <tableColumns count="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}" name="Table1" displayName="Table1" ref="A1:W6" totalsRowShown="0">
+  <autoFilter ref="A1:W6" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
+  <tableColumns count="23">
     <tableColumn id="1" xr3:uid="{C73E51D0-1842-42F3-9C00-F0DBD2E661BE}" name="Unit"/>
     <tableColumn id="2" xr3:uid="{FA8BE796-DE15-407E-8998-92C973AE35A4}" name="Input1"/>
     <tableColumn id="3" xr3:uid="{168877A6-E181-4446-9569-F36E8CEB8908}" name="Input2"/>
@@ -298,16 +316,19 @@
     <tableColumn id="10" xr3:uid="{ACDE4024-BCA2-4145-B3BC-1A5A08F3EA7D}" name="Relation_Out_Out"/>
     <tableColumn id="11" xr3:uid="{8AEC88A1-B64A-43A2-AC89-3B27AB4ACAD7}" name="Cost_invest"/>
     <tableColumn id="12" xr3:uid="{F1A83AF0-CF23-4B00-9076-4E28DF8DAFD3}" name="fom_cost"/>
-    <tableColumn id="13" xr3:uid="{AD4231E3-CB94-4597-81A2-E13C044BBD2D}" name="vom_cost"/>
+    <tableColumn id="13" xr3:uid="{AD4231E3-CB94-4597-81A2-E13C044BBD2D}" name="vom_cost_Input1"/>
+    <tableColumn id="21" xr3:uid="{400CD12D-8ADA-4557-B7CA-1464809EAFF0}" name="vom_cost_Input2"/>
+    <tableColumn id="22" xr3:uid="{3FA572AD-B473-45F7-A244-2DF38E57A2D3}" name="vom_cost_Output1"/>
+    <tableColumn id="23" xr3:uid="{1F97C2CD-E522-4842-8E10-F9B9566A6723}" name="vom_cost_Output2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{856854C3-DC05-4AB8-91B8-0E52D9C11DBC}" name="Table13" displayName="Table13" ref="A1:V5" totalsRowShown="0">
-  <autoFilter ref="A1:V5" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
-  <tableColumns count="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{856854C3-DC05-4AB8-91B8-0E52D9C11DBC}" name="Table13" displayName="Table13" ref="A1:W5" totalsRowShown="0">
+  <autoFilter ref="A1:W5" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
+  <tableColumns count="23">
     <tableColumn id="1" xr3:uid="{26B0CA71-1EA9-44CF-8E6D-31054ECA99A6}" name="Connection"/>
     <tableColumn id="2" xr3:uid="{587ADBB8-7B68-42BE-A14F-535C6116E5EA}" name="Input1"/>
     <tableColumn id="3" xr3:uid="{0B221EED-10BC-4C34-AC5E-37A826B1E8AE}" name="Input2"/>
@@ -329,7 +350,8 @@
     <tableColumn id="23" xr3:uid="{C3B5D3DD-6B9E-4750-8098-2BDCA6D4F76B}" name="Relation_Out_In"/>
     <tableColumn id="11" xr3:uid="{ADDA3F91-13EA-44FD-BDAD-129E45FF1B77}" name="Cost_invest"/>
     <tableColumn id="12" xr3:uid="{19693C8E-93B1-45BA-838A-11FFE3971C45}" name="fom_cost"/>
-    <tableColumn id="13" xr3:uid="{9A50D747-7636-48C7-AEA4-AC76517E91C7}" name="vom_cost"/>
+    <tableColumn id="13" xr3:uid="{9A50D747-7636-48C7-AEA4-AC76517E91C7}" name="vom_cost_input1"/>
+    <tableColumn id="21" xr3:uid="{EC2CC790-C17D-4744-A981-3984808E5B33}" name="vom_cost_output1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -653,10 +675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
-  <dimension ref="A1:T6"/>
+  <dimension ref="A1:W6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T28" sqref="T28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -680,7 +702,7 @@
     <col min="20" max="20" width="11.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -739,10 +761,19 @@
         <v>54</v>
       </c>
       <c r="T1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+        <v>57</v>
+      </c>
+      <c r="U1" t="s">
+        <v>58</v>
+      </c>
+      <c r="V1" t="s">
+        <v>59</v>
+      </c>
+      <c r="W1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -759,7 +790,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -788,7 +819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -808,7 +839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -829,7 +860,7 @@
         <v>1.2578616352201257</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -879,10 +910,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C870BDA0-9E4C-481D-87BE-9D47789809C8}">
-  <dimension ref="A1:V5"/>
+  <dimension ref="A1:W5"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="U1" sqref="U1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="V8" sqref="V8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -908,7 +939,7 @@
     <col min="22" max="22" width="11.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>37</v>
       </c>
@@ -973,10 +1004,13 @@
         <v>54</v>
       </c>
       <c r="V1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+      <c r="W1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -1026,7 +1060,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -1064,7 +1098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -1099,7 +1133,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
separate object node definition
</commit_message>
<xml_diff>
--- a/spine_projects/01_input_data/01_input_raw/Model_Data_Base.xlsx
+++ b/spine_projects/01_input_data/01_input_raw/Model_Data_Base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98F524D2-D14F-43F9-A9E1-97B76DBB6870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF60D57A-84DD-4337-93E7-427775834AA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-3810" yWindow="-20460" windowWidth="28800" windowHeight="15225" activeTab="1" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="59">
   <si>
     <t>Unit</t>
   </si>
@@ -205,9 +205,6 @@
     <t>fom_cost</t>
   </si>
   <si>
-    <t>vom_cost_Input1</t>
-  </si>
-  <si>
     <t>vom_cost_Input2</t>
   </si>
   <si>
@@ -215,6 +212,9 @@
   </si>
   <si>
     <t>vom_cost_Output2</t>
+  </si>
+  <si>
+    <t>vom_cost_Input12</t>
   </si>
 </sst>
 </file>
@@ -288,9 +288,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}" name="Table1" displayName="Table1" ref="A1:W6" totalsRowShown="0">
-  <autoFilter ref="A1:W6" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
-  <tableColumns count="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}" name="Table1" displayName="Table1" ref="A1:X6" totalsRowShown="0">
+  <autoFilter ref="A1:X6" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
+  <tableColumns count="24">
     <tableColumn id="1" xr3:uid="{C73E51D0-1842-42F3-9C00-F0DBD2E661BE}" name="Unit"/>
     <tableColumn id="2" xr3:uid="{FA8BE796-DE15-407E-8998-92C973AE35A4}" name="Input1"/>
     <tableColumn id="3" xr3:uid="{168877A6-E181-4446-9569-F36E8CEB8908}" name="Input2"/>
@@ -310,7 +310,8 @@
     <tableColumn id="10" xr3:uid="{ACDE4024-BCA2-4145-B3BC-1A5A08F3EA7D}" name="Relation_Out_Out"/>
     <tableColumn id="11" xr3:uid="{8AEC88A1-B64A-43A2-AC89-3B27AB4ACAD7}" name="Cost_invest"/>
     <tableColumn id="12" xr3:uid="{F1A83AF0-CF23-4B00-9076-4E28DF8DAFD3}" name="fom_cost"/>
-    <tableColumn id="13" xr3:uid="{AD4231E3-CB94-4597-81A2-E13C044BBD2D}" name="vom_cost_Input1"/>
+    <tableColumn id="24" xr3:uid="{4D171E04-3F62-4131-BD43-B8A8D03B8530}" name="vom_cost"/>
+    <tableColumn id="13" xr3:uid="{AD4231E3-CB94-4597-81A2-E13C044BBD2D}" name="vom_cost_Input12"/>
     <tableColumn id="21" xr3:uid="{400CD12D-8ADA-4557-B7CA-1464809EAFF0}" name="vom_cost_Input2"/>
     <tableColumn id="22" xr3:uid="{3FA572AD-B473-45F7-A244-2DF38E57A2D3}" name="vom_cost_Output1"/>
     <tableColumn id="23" xr3:uid="{1F97C2CD-E522-4842-8E10-F9B9566A6723}" name="vom_cost_Output2"/>
@@ -320,9 +321,9 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{856854C3-DC05-4AB8-91B8-0E52D9C11DBC}" name="Table13" displayName="Table13" ref="A1:Y5" totalsRowShown="0">
-  <autoFilter ref="A1:Y5" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
-  <tableColumns count="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{856854C3-DC05-4AB8-91B8-0E52D9C11DBC}" name="Table13" displayName="Table13" ref="A1:Z5" totalsRowShown="0">
+  <autoFilter ref="A1:Z5" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
+  <tableColumns count="26">
     <tableColumn id="1" xr3:uid="{26B0CA71-1EA9-44CF-8E6D-31054ECA99A6}" name="Connection"/>
     <tableColumn id="2" xr3:uid="{587ADBB8-7B68-42BE-A14F-535C6116E5EA}" name="Input1"/>
     <tableColumn id="3" xr3:uid="{0B221EED-10BC-4C34-AC5E-37A826B1E8AE}" name="Input2"/>
@@ -344,7 +345,8 @@
     <tableColumn id="23" xr3:uid="{C3B5D3DD-6B9E-4750-8098-2BDCA6D4F76B}" name="Relation_Out_In"/>
     <tableColumn id="11" xr3:uid="{ADDA3F91-13EA-44FD-BDAD-129E45FF1B77}" name="Cost_invest"/>
     <tableColumn id="12" xr3:uid="{19693C8E-93B1-45BA-838A-11FFE3971C45}" name="fom_cost"/>
-    <tableColumn id="13" xr3:uid="{9A50D747-7636-48C7-AEA4-AC76517E91C7}" name="vom_cost_Input1"/>
+    <tableColumn id="26" xr3:uid="{4DB0EE1D-1F20-454E-A875-16374060A367}" name="vom_cost"/>
+    <tableColumn id="13" xr3:uid="{9A50D747-7636-48C7-AEA4-AC76517E91C7}" name="vom_cost_Input12"/>
     <tableColumn id="21" xr3:uid="{EC2CC790-C17D-4744-A981-3984808E5B33}" name="vom_cost_Input2"/>
     <tableColumn id="24" xr3:uid="{41B338E4-2058-41E9-8000-97D77450FBC3}" name="vom_cost_Output1"/>
     <tableColumn id="25" xr3:uid="{DDAFCF0A-1EF1-4B7B-9742-01F9FA7A22E5}" name="vom_cost_Output2"/>
@@ -671,10 +673,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
-  <dimension ref="A1:W6"/>
+  <dimension ref="A1:X6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T1" sqref="T1:W1"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -695,10 +697,11 @@
     <col min="17" max="17" width="18.81640625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="12.7265625" customWidth="1"/>
     <col min="19" max="19" width="11" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11" customWidth="1"/>
+    <col min="21" max="21" width="11.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -757,19 +760,22 @@
         <v>54</v>
       </c>
       <c r="T1" t="s">
+        <v>53</v>
+      </c>
+      <c r="U1" t="s">
+        <v>58</v>
+      </c>
+      <c r="V1" t="s">
         <v>55</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>56</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>57</v>
       </c>
-      <c r="W1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -786,7 +792,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -814,8 +820,11 @@
       <c r="T3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="U3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -835,7 +844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -856,7 +865,7 @@
         <v>1.2578616352201257</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -906,10 +915,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C870BDA0-9E4C-481D-87BE-9D47789809C8}">
-  <dimension ref="A1:Y5"/>
+  <dimension ref="A1:Z5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W10" sqref="W10"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="U18" sqref="U18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -932,10 +941,11 @@
     <col min="19" max="19" width="18.81640625" customWidth="1"/>
     <col min="20" max="20" width="12.7265625" customWidth="1"/>
     <col min="21" max="21" width="11" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11" customWidth="1"/>
+    <col min="23" max="23" width="11.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>37</v>
       </c>
@@ -1000,19 +1010,22 @@
         <v>54</v>
       </c>
       <c r="V1" t="s">
+        <v>53</v>
+      </c>
+      <c r="W1" t="s">
+        <v>58</v>
+      </c>
+      <c r="X1" t="s">
         <v>55</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>56</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>57</v>
       </c>
-      <c r="Y1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -1062,7 +1075,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -1099,8 +1112,11 @@
       <c r="V3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="W3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -1135,7 +1151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
update data prep script
</commit_message>
<xml_diff>
--- a/spine_projects/01_input_data/01_input_raw/Model_Data_Base.xlsx
+++ b/spine_projects/01_input_data/01_input_raw/Model_Data_Base.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF60D57A-84DD-4337-93E7-427775834AA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C3BAB7B-BB92-4D39-AFC8-9D560C731FAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3810" yWindow="-20460" windowWidth="28800" windowHeight="15225" activeTab="1" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-5070" yWindow="-21720" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -214,7 +214,7 @@
     <t>vom_cost_Output2</t>
   </si>
   <si>
-    <t>vom_cost_Input12</t>
+    <t>vom_cost_Input1</t>
   </si>
 </sst>
 </file>
@@ -311,7 +311,7 @@
     <tableColumn id="11" xr3:uid="{8AEC88A1-B64A-43A2-AC89-3B27AB4ACAD7}" name="Cost_invest"/>
     <tableColumn id="12" xr3:uid="{F1A83AF0-CF23-4B00-9076-4E28DF8DAFD3}" name="fom_cost"/>
     <tableColumn id="24" xr3:uid="{4D171E04-3F62-4131-BD43-B8A8D03B8530}" name="vom_cost"/>
-    <tableColumn id="13" xr3:uid="{AD4231E3-CB94-4597-81A2-E13C044BBD2D}" name="vom_cost_Input12"/>
+    <tableColumn id="13" xr3:uid="{AD4231E3-CB94-4597-81A2-E13C044BBD2D}" name="vom_cost_Input1"/>
     <tableColumn id="21" xr3:uid="{400CD12D-8ADA-4557-B7CA-1464809EAFF0}" name="vom_cost_Input2"/>
     <tableColumn id="22" xr3:uid="{3FA572AD-B473-45F7-A244-2DF38E57A2D3}" name="vom_cost_Output1"/>
     <tableColumn id="23" xr3:uid="{1F97C2CD-E522-4842-8E10-F9B9566A6723}" name="vom_cost_Output2"/>
@@ -346,7 +346,7 @@
     <tableColumn id="11" xr3:uid="{ADDA3F91-13EA-44FD-BDAD-129E45FF1B77}" name="Cost_invest"/>
     <tableColumn id="12" xr3:uid="{19693C8E-93B1-45BA-838A-11FFE3971C45}" name="fom_cost"/>
     <tableColumn id="26" xr3:uid="{4DB0EE1D-1F20-454E-A875-16374060A367}" name="vom_cost"/>
-    <tableColumn id="13" xr3:uid="{9A50D747-7636-48C7-AEA4-AC76517E91C7}" name="vom_cost_Input12"/>
+    <tableColumn id="13" xr3:uid="{9A50D747-7636-48C7-AEA4-AC76517E91C7}" name="vom_cost_Input1"/>
     <tableColumn id="21" xr3:uid="{EC2CC790-C17D-4744-A981-3984808E5B33}" name="vom_cost_Input2"/>
     <tableColumn id="24" xr3:uid="{41B338E4-2058-41E9-8000-97D77450FBC3}" name="vom_cost_Output1"/>
     <tableColumn id="25" xr3:uid="{DDAFCF0A-1EF1-4B7B-9742-01F9FA7A22E5}" name="vom_cost_Output2"/>
@@ -676,7 +676,7 @@
   <dimension ref="A1:X6"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="T4" sqref="T4"/>
+      <selection activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -918,7 +918,7 @@
   <dimension ref="A1:Z5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="U18" sqref="U18"/>
+      <selection activeCell="V1" sqref="V1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
test new vom_cost implementation
</commit_message>
<xml_diff>
--- a/spine_projects/01_input_data/01_input_raw/Model_Data_Base.xlsx
+++ b/spine_projects/01_input_data/01_input_raw/Model_Data_Base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7655466-D058-4271-A3BE-1CCD753849D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14DC064E-F0C1-4084-8963-BB76C150F61D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-5070" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="59">
   <si>
     <t>Unit</t>
   </si>
@@ -321,9 +321,9 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{856854C3-DC05-4AB8-91B8-0E52D9C11DBC}" name="Table13" displayName="Table13" ref="A1:Z5" totalsRowShown="0">
-  <autoFilter ref="A1:Z5" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
-  <tableColumns count="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{856854C3-DC05-4AB8-91B8-0E52D9C11DBC}" name="Table13" displayName="Table13" ref="A1:Y5" totalsRowShown="0">
+  <autoFilter ref="A1:Y5" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
+  <tableColumns count="25">
     <tableColumn id="1" xr3:uid="{26B0CA71-1EA9-44CF-8E6D-31054ECA99A6}" name="Connection"/>
     <tableColumn id="2" xr3:uid="{587ADBB8-7B68-42BE-A14F-535C6116E5EA}" name="Input1"/>
     <tableColumn id="3" xr3:uid="{0B221EED-10BC-4C34-AC5E-37A826B1E8AE}" name="Input2"/>
@@ -345,7 +345,6 @@
     <tableColumn id="23" xr3:uid="{C3B5D3DD-6B9E-4750-8098-2BDCA6D4F76B}" name="Relation_Out_In"/>
     <tableColumn id="11" xr3:uid="{ADDA3F91-13EA-44FD-BDAD-129E45FF1B77}" name="Cost_invest"/>
     <tableColumn id="12" xr3:uid="{19693C8E-93B1-45BA-838A-11FFE3971C45}" name="fom_cost"/>
-    <tableColumn id="26" xr3:uid="{4DB0EE1D-1F20-454E-A875-16374060A367}" name="vom_cost"/>
     <tableColumn id="13" xr3:uid="{9A50D747-7636-48C7-AEA4-AC76517E91C7}" name="vom_cost_Input1"/>
     <tableColumn id="21" xr3:uid="{EC2CC790-C17D-4744-A981-3984808E5B33}" name="vom_cost_Input2"/>
     <tableColumn id="24" xr3:uid="{41B338E4-2058-41E9-8000-97D77450FBC3}" name="vom_cost_Output1"/>
@@ -676,7 +675,7 @@
   <dimension ref="A1:X6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+      <selection activeCell="R23" sqref="R23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -820,6 +819,9 @@
       <c r="Q3">
         <v>1</v>
       </c>
+      <c r="U3">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -912,10 +914,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C870BDA0-9E4C-481D-87BE-9D47789809C8}">
-  <dimension ref="A1:Z5"/>
+  <dimension ref="A1:Y5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="W4" sqref="W4"/>
+      <selection activeCell="V3" sqref="V3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -938,11 +940,10 @@
     <col min="19" max="19" width="18.81640625" customWidth="1"/>
     <col min="20" max="20" width="12.7265625" customWidth="1"/>
     <col min="21" max="21" width="11" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11" customWidth="1"/>
-    <col min="23" max="23" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>37</v>
       </c>
@@ -1007,22 +1008,19 @@
         <v>54</v>
       </c>
       <c r="V1" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="W1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="X1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="Y1" t="s">
-        <v>56</v>
-      </c>
-      <c r="Z1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -1072,7 +1070,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -1107,7 +1105,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -1142,7 +1140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
Added fom costs and adjusted mapping
also adjusted "has_state" to achieve "true" instead of "True" to avoid read in errors
</commit_message>
<xml_diff>
--- a/spine_projects/01_input_data/01_input_raw/Model_Data_Base.xlsx
+++ b/spine_projects/01_input_data/01_input_raw/Model_Data_Base.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/dahe23af_student_cbs_dk/Documents/Dokumente/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14DC064E-F0C1-4084-8963-BB76C150F61D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{14DC064E-F0C1-4084-8963-BB76C150F61D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8838214B-CD8D-48D5-9A48-8474320ADEEC}"/>
   <bookViews>
-    <workbookView xWindow="-5070" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-750" yWindow="-14835" windowWidth="17745" windowHeight="10890" activeTab="2" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -674,7 +674,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
   <dimension ref="A1:X6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R23" sqref="R23"/>
     </sheetView>
   </sheetViews>
@@ -1182,8 +1182,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{981CFA5E-60F3-446F-A856-2FA65B76879A}">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1277,6 +1277,11 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D5" xr:uid="{5D5BF415-E056-4F96-A602-1B73CD7FB1B5}">
+      <formula1>"true, false"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
add min downtime and unit_on_cost to input data
</commit_message>
<xml_diff>
--- a/spine_projects/01_input_data/01_input_raw/Model_Data_Base.xlsx
+++ b/spine_projects/01_input_data/01_input_raw/Model_Data_Base.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/dahe23af_student_cbs_dk/Documents/Dokumente/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{14DC064E-F0C1-4084-8963-BB76C150F61D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8838214B-CD8D-48D5-9A48-8474320ADEEC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B6D3EA2-E6FD-4792-AAC2-943631E93881}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-750" yWindow="-14835" windowWidth="17745" windowHeight="10890" activeTab="2" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-5070" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="62">
   <si>
     <t>Unit</t>
   </si>
@@ -215,6 +215,15 @@
   </si>
   <si>
     <t>vom_cost_Input1</t>
+  </si>
+  <si>
+    <t>min_down_time</t>
+  </si>
+  <si>
+    <t>unit_on_cost</t>
+  </si>
+  <si>
+    <t>0.0000001</t>
   </si>
 </sst>
 </file>
@@ -288,9 +297,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}" name="Table1" displayName="Table1" ref="A1:X6" totalsRowShown="0">
-  <autoFilter ref="A1:X6" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
-  <tableColumns count="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}" name="Table1" displayName="Table1" ref="A1:Y6" totalsRowShown="0">
+  <autoFilter ref="A1:Y6" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
+  <tableColumns count="25">
     <tableColumn id="1" xr3:uid="{C73E51D0-1842-42F3-9C00-F0DBD2E661BE}" name="Unit"/>
     <tableColumn id="2" xr3:uid="{FA8BE796-DE15-407E-8998-92C973AE35A4}" name="Input1"/>
     <tableColumn id="3" xr3:uid="{168877A6-E181-4446-9569-F36E8CEB8908}" name="Input2"/>
@@ -304,11 +313,12 @@
     <tableColumn id="17" xr3:uid="{6408F114-841E-472E-92F5-7B63FF1B66F4}" name="Cap_Output_1_max"/>
     <tableColumn id="18" xr3:uid="{541C17F0-C020-47FE-9DA4-DB76D7416668}" name="Cap_Output2_existing"/>
     <tableColumn id="19" xr3:uid="{D6FEE63D-DC89-4D1A-9708-5E7C70FD5793}" name="Cap_Output2_max"/>
-    <tableColumn id="8" xr3:uid="{5F719CEE-A0F7-452C-B82C-E739C5FED49B}" name="Efficency"/>
+    <tableColumn id="8" xr3:uid="{5F719CEE-A0F7-452C-B82C-E739C5FED49B}" name="min_down_time"/>
     <tableColumn id="9" xr3:uid="{50F936EF-D32C-4938-8FCA-291A6A3E82E6}" name="Relation_In_In"/>
     <tableColumn id="20" xr3:uid="{84C680FD-12EA-4AE2-A238-57453A3D8C12}" name="Relation_In_Out"/>
     <tableColumn id="10" xr3:uid="{ACDE4024-BCA2-4145-B3BC-1A5A08F3EA7D}" name="Relation_Out_Out"/>
     <tableColumn id="11" xr3:uid="{8AEC88A1-B64A-43A2-AC89-3B27AB4ACAD7}" name="Cost_invest"/>
+    <tableColumn id="25" xr3:uid="{95F69D80-80E7-42BD-B42F-59F3C3DC485B}" name="unit_on_cost"/>
     <tableColumn id="12" xr3:uid="{F1A83AF0-CF23-4B00-9076-4E28DF8DAFD3}" name="fom_cost"/>
     <tableColumn id="24" xr3:uid="{4D171E04-3F62-4131-BD43-B8A8D03B8530}" name="vom_cost"/>
     <tableColumn id="13" xr3:uid="{AD4231E3-CB94-4597-81A2-E13C044BBD2D}" name="vom_cost_Input1"/>
@@ -672,10 +682,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
-  <dimension ref="A1:X6"/>
+  <dimension ref="A1:Y6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R23" sqref="R23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -694,13 +704,13 @@
     <col min="15" max="15" width="15.6328125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="17.1796875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.7265625" customWidth="1"/>
-    <col min="19" max="19" width="11" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11" customWidth="1"/>
-    <col min="21" max="21" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="12.7265625" customWidth="1"/>
+    <col min="20" max="20" width="11" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11" customWidth="1"/>
+    <col min="22" max="22" width="11.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -741,7 +751,7 @@
         <v>35</v>
       </c>
       <c r="N1" t="s">
-        <v>7</v>
+        <v>59</v>
       </c>
       <c r="O1" t="s">
         <v>39</v>
@@ -756,25 +766,28 @@
         <v>8</v>
       </c>
       <c r="S1" t="s">
+        <v>60</v>
+      </c>
+      <c r="T1" t="s">
         <v>54</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>53</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>58</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>55</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>56</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -787,11 +800,11 @@
       <c r="K2">
         <v>304</v>
       </c>
-      <c r="S2">
+      <c r="T2">
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -819,11 +832,11 @@
       <c r="Q3">
         <v>1</v>
       </c>
-      <c r="U3">
+      <c r="V3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -843,7 +856,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -863,8 +876,11 @@
         <f>1/0.795</f>
         <v>1.2578616352201257</v>
       </c>
+      <c r="S5" t="s">
+        <v>61</v>
+      </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -891,6 +907,9 @@
       </c>
       <c r="M6">
         <v>10</v>
+      </c>
+      <c r="N6">
+        <v>48</v>
       </c>
       <c r="O6">
         <v>1</v>
@@ -1182,7 +1201,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{981CFA5E-60F3-446F-A856-2FA65B76879A}">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
integrate ramping into data prep and input data
</commit_message>
<xml_diff>
--- a/spine_projects/01_input_data/01_input_raw/Model_Data_Base.xlsx
+++ b/spine_projects/01_input_data/01_input_raw/Model_Data_Base.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B6D3EA2-E6FD-4792-AAC2-943631E93881}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC38734D-A4AA-4898-8732-98E602FACD4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5070" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-3300" yWindow="-19950" windowWidth="28800" windowHeight="15225" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="66">
   <si>
     <t>Unit</t>
   </si>
@@ -224,6 +224,18 @@
   </si>
   <si>
     <t>0.0000001</t>
+  </si>
+  <si>
+    <t>ramp_up_Output1</t>
+  </si>
+  <si>
+    <t>ramp_up_Output2</t>
+  </si>
+  <si>
+    <t>ramp_down_Output2</t>
+  </si>
+  <si>
+    <t>ramp_down_Output1</t>
   </si>
 </sst>
 </file>
@@ -297,9 +309,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}" name="Table1" displayName="Table1" ref="A1:Y6" totalsRowShown="0">
-  <autoFilter ref="A1:Y6" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
-  <tableColumns count="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}" name="Table1" displayName="Table1" ref="A1:AC6" totalsRowShown="0">
+  <autoFilter ref="A1:AC6" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
+  <tableColumns count="29">
     <tableColumn id="1" xr3:uid="{C73E51D0-1842-42F3-9C00-F0DBD2E661BE}" name="Unit"/>
     <tableColumn id="2" xr3:uid="{FA8BE796-DE15-407E-8998-92C973AE35A4}" name="Input1"/>
     <tableColumn id="3" xr3:uid="{168877A6-E181-4446-9569-F36E8CEB8908}" name="Input2"/>
@@ -314,6 +326,10 @@
     <tableColumn id="18" xr3:uid="{541C17F0-C020-47FE-9DA4-DB76D7416668}" name="Cap_Output2_existing"/>
     <tableColumn id="19" xr3:uid="{D6FEE63D-DC89-4D1A-9708-5E7C70FD5793}" name="Cap_Output2_max"/>
     <tableColumn id="8" xr3:uid="{5F719CEE-A0F7-452C-B82C-E739C5FED49B}" name="min_down_time"/>
+    <tableColumn id="26" xr3:uid="{D0F85E7B-D704-45A0-BE99-26E3A1F08634}" name="ramp_up_Output1"/>
+    <tableColumn id="28" xr3:uid="{EBC4610B-47F0-44E3-8543-664851FC473C}" name="ramp_up_Output2"/>
+    <tableColumn id="27" xr3:uid="{DC89C4F2-3857-45F2-B4A0-642F9C1613A6}" name="ramp_down_Output1"/>
+    <tableColumn id="29" xr3:uid="{5A66563E-85FF-4FFA-9DB7-EAC64F37E721}" name="ramp_down_Output2"/>
     <tableColumn id="9" xr3:uid="{50F936EF-D32C-4938-8FCA-291A6A3E82E6}" name="Relation_In_In"/>
     <tableColumn id="20" xr3:uid="{84C680FD-12EA-4AE2-A238-57453A3D8C12}" name="Relation_In_Out"/>
     <tableColumn id="10" xr3:uid="{ACDE4024-BCA2-4145-B3BC-1A5A08F3EA7D}" name="Relation_Out_Out"/>
@@ -682,10 +698,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
-  <dimension ref="A1:Y6"/>
+  <dimension ref="A1:AC6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -700,17 +716,17 @@
     <col min="11" max="11" width="20.08984375" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="21.90625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="19" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="10.54296875" customWidth="1"/>
-    <col min="15" max="15" width="15.6328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="12.7265625" customWidth="1"/>
-    <col min="20" max="20" width="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11" customWidth="1"/>
-    <col min="22" max="22" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="14" max="18" width="10.54296875" customWidth="1"/>
+    <col min="19" max="19" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="12.7265625" customWidth="1"/>
+    <col min="24" max="24" width="11" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11" customWidth="1"/>
+    <col min="26" max="26" width="11.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -754,40 +770,52 @@
         <v>59</v>
       </c>
       <c r="O1" t="s">
+        <v>62</v>
+      </c>
+      <c r="P1" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>65</v>
+      </c>
+      <c r="R1" t="s">
+        <v>64</v>
+      </c>
+      <c r="S1" t="s">
         <v>39</v>
       </c>
-      <c r="P1" t="s">
+      <c r="T1" t="s">
         <v>38</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="U1" t="s">
         <v>40</v>
       </c>
-      <c r="R1" t="s">
+      <c r="V1" t="s">
         <v>8</v>
       </c>
-      <c r="S1" t="s">
+      <c r="W1" t="s">
         <v>60</v>
       </c>
-      <c r="T1" t="s">
+      <c r="X1" t="s">
         <v>54</v>
       </c>
-      <c r="U1" t="s">
+      <c r="Y1" t="s">
         <v>53</v>
       </c>
-      <c r="V1" t="s">
+      <c r="Z1" t="s">
         <v>58</v>
       </c>
-      <c r="W1" t="s">
+      <c r="AA1" t="s">
         <v>55</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AB1" t="s">
         <v>56</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AC1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -800,11 +828,11 @@
       <c r="K2">
         <v>304</v>
       </c>
-      <c r="T2">
+      <c r="X2">
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -826,17 +854,17 @@
       <c r="G3">
         <v>52</v>
       </c>
-      <c r="O3">
+      <c r="S3">
         <v>4.7614285714285716</v>
       </c>
-      <c r="Q3">
+      <c r="U3">
         <v>1</v>
       </c>
-      <c r="V3">
+      <c r="Z3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -852,11 +880,11 @@
       <c r="K4">
         <v>100</v>
       </c>
-      <c r="P4">
+      <c r="T4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -872,15 +900,12 @@
       <c r="J5">
         <v>52</v>
       </c>
-      <c r="P5">
+      <c r="T5">
         <f>1/0.795</f>
         <v>1.2578616352201257</v>
       </c>
-      <c r="S5" t="s">
-        <v>61</v>
-      </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -912,14 +937,23 @@
         <v>48</v>
       </c>
       <c r="O6">
+        <v>0.5</v>
+      </c>
+      <c r="Q6">
+        <v>0.5</v>
+      </c>
+      <c r="S6">
         <v>1</v>
       </c>
-      <c r="P6">
+      <c r="T6">
         <f>1/0.96</f>
         <v>1.0416666666666667</v>
       </c>
-      <c r="Q6">
+      <c r="U6">
         <v>4</v>
+      </c>
+      <c r="W6" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>